<commit_message>
print stacked bar chart with error bars
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChristianKrenslehner\Desktop\temp\python_pandas_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4307995E-C41B-4152-BC35-CC11670FFC6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E11AEED-47D3-4211-8D76-A4F4E0BDD27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{472E3A0B-3A28-45AE-B75A-9637174FA5AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{472E3A0B-3A28-45AE-B75A-9637174FA5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_one" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Hour</t>
   </si>
@@ -428,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{347A4962-13C0-4BD5-88A0-08DE7B1CA582}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,220 +1066,610 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65BC2EE-2FA8-4F5C-AF00-3975BA868386}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <f>B2*0.9</f>
+        <v>27</v>
+      </c>
+      <c r="E2">
+        <f>AVERAGE(B2:D2)</f>
+        <v>25.666666666666668</v>
+      </c>
+      <c r="F2">
+        <f>STDEVA(B2:D2)</f>
+        <v>5.1316014394468876</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D26" si="0">B3*0.9</f>
+        <v>26.1</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E26" si="1">AVERAGE(B3:D3)</f>
+        <v>25.366666666666664</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F26" si="2">STDEVA(B3:D3)</f>
+        <v>4.0501028793517744</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>25.2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>24.400000000000002</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>4.0595566260368763</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>24.3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>24.099999999999998</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>3.0049958402633394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>23.400000000000002</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>23.133333333333336</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>3.0088757590391086</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>22.633333333333336</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>2.3028967265887843</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>21.6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1.8330302779823364</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>20.7</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>21.366666666666664</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>1.4224392195567919</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>19.8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>20.733333333333334</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>1.1372481406154653</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>18.900000000000002</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>20.099999999999998</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>1.0816653826391953</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>19.466666666666665</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>1.2858201014657269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>17.100000000000001</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>18.833333333333332</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>1.6563010998406444</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>16.2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>18.2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>2.1071307505705477</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>15.3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>17.566666666666666</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>2.5967928938082996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>14.4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>16.933333333333334</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>3.1069813860616167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>16.3</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>3.6290494623248053</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>12.6</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>15.666666666666666</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>4.1585253796668473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>11.700000000000001</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>15.033333333333333</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>4.6929024423413335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>10.8</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>14.4</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>5.230678732248804</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>9.9</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>13.766666666666666</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>5.7709040308545543</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>13.133333333333333</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>6.312949653952054</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>8.1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>6.8563838865687785</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>7.2</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>11.866666666666667</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>7.4009008460682209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>6.3</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>11.233333333333333</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>7.9462779546988775</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>34</v>
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>5.4</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>10.6</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>8.4923494982248595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add stub for clustered_plot class
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChristianKrenslehner\Desktop\temp\python_pandas_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E11AEED-47D3-4211-8D76-A4F4E0BDD27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF3D5D1-48AB-4987-95B2-F8F6259E0AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{472E3A0B-3A28-45AE-B75A-9637174FA5AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{472E3A0B-3A28-45AE-B75A-9637174FA5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_one" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Hour</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Deviation</t>
+  </si>
+  <si>
+    <t>MaxTemperature1</t>
+  </si>
+  <si>
+    <t>MaxTemperature2</t>
+  </si>
+  <si>
+    <t>MaxTemperature3</t>
+  </si>
+  <si>
+    <t>DiffMaxAvgTemperature1</t>
   </si>
 </sst>
 </file>
@@ -426,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{347A4962-13C0-4BD5-88A0-08DE7B1CA582}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,9 +449,11 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="7" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,8 +472,26 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -482,8 +514,32 @@
         <f>STDEVA(B2:D2)</f>
         <v>1.5275252316519465</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f>MAX(B2:B26)</f>
+        <v>44</v>
+      </c>
+      <c r="H2">
+        <f>MAX(C2:C26)</f>
+        <v>45</v>
+      </c>
+      <c r="I2">
+        <f>MAX(D2:D26)</f>
+        <v>39.6</v>
+      </c>
+      <c r="J2">
+        <f>ABS(G2-$E$2)</f>
+        <v>24.333333333333332</v>
+      </c>
+      <c r="K2">
+        <f>ABS(H2-$E$2)</f>
+        <v>25.333333333333332</v>
+      </c>
+      <c r="L2">
+        <f>ABS(I2-$E$2)</f>
+        <v>19.933333333333334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -507,7 +563,7 @@
         <v>1.5821925715074412</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -531,7 +587,7 @@
         <v>1.6370705543744897</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -555,7 +611,7 @@
         <v>1.6921386861996077</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -579,7 +635,7 @@
         <v>1.7473789896108201</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -603,7 +659,7 @@
         <v>1.8027756377319946</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -627,7 +683,7 @@
         <v>1.8583146486355127</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -651,7 +707,7 @@
         <v>1.913983629327412</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -675,7 +731,7 @@
         <v>1.9697715603592214</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -699,7 +755,7 @@
         <v>2.0256686138984654</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -723,7 +779,7 @@
         <v>2.0816659994661331</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -747,7 +803,7 @@
         <v>2.1377558326431938</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -771,7 +827,7 @@
         <v>2.1939310229205775</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -795,7 +851,7 @@
         <v>2.2501851775650232</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1066,18 +1122,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65BC2EE-2FA8-4F5C-AF00-3975BA868386}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="11" max="12" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1096,8 +1156,26 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1119,8 +1197,32 @@
         <f>STDEVA(B2:D2)</f>
         <v>5.1316014394468876</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f>MAX(B2:B26)</f>
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <f>MAX(C2:C26)</f>
+        <v>21</v>
+      </c>
+      <c r="I2">
+        <f>MAX(D2:D26)</f>
+        <v>27</v>
+      </c>
+      <c r="J2">
+        <f>ABS(G2-$E$2)</f>
+        <v>4.3333333333333321</v>
+      </c>
+      <c r="K2">
+        <f>ABS(H2-$E$2)</f>
+        <v>4.6666666666666679</v>
+      </c>
+      <c r="L2">
+        <f>ABS(I2-$E$2)</f>
+        <v>1.3333333333333321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1143,7 +1245,7 @@
         <v>4.0501028793517744</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1166,7 +1268,7 @@
         <v>4.0595566260368763</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1189,7 +1291,7 @@
         <v>3.0049958402633394</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1212,7 +1314,7 @@
         <v>3.0088757590391086</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1235,7 +1337,7 @@
         <v>2.3028967265887843</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1258,7 +1360,7 @@
         <v>1.8330302779823364</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1281,7 +1383,7 @@
         <v>1.4224392195567919</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1304,7 +1406,7 @@
         <v>1.1372481406154653</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1327,7 +1429,7 @@
         <v>1.0816653826391953</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1350,7 +1452,7 @@
         <v>1.2858201014657269</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1373,7 +1475,7 @@
         <v>1.6563010998406444</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1396,7 +1498,7 @@
         <v>2.1071307505705477</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1419,7 +1521,7 @@
         <v>2.5967928938082996</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>

</xml_diff>